<commit_message>
First approach to Hierarchical Clustering
</commit_message>
<xml_diff>
--- a/Datasets/VarCovid.xlsx
+++ b/Datasets/VarCovid.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/davpero/ine_sg_difusion_explica_datasets/Datasets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E983966-9FB0-7F44-AC6B-05EE1BAD0EF2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F89A373C-2945-BE4E-A84F-8AEB794322F4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="780" yWindow="1520" windowWidth="26780" windowHeight="16080" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="102">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="103">
   <si>
     <t>2020SM53</t>
   </si>
@@ -45,12 +45,6 @@
     <t>ccaa</t>
   </si>
   <si>
-    <t>Andalucía</t>
-  </si>
-  <si>
-    <t>Aragón</t>
-  </si>
-  <si>
     <t>Asturias, Principado de</t>
   </si>
   <si>
@@ -63,15 +57,9 @@
     <t>Cantabria</t>
   </si>
   <si>
-    <t>Castilla y León</t>
-  </si>
-  <si>
     <t>Castilla - La Mancha</t>
   </si>
   <si>
-    <t>Cataluña</t>
-  </si>
-  <si>
     <t>Comunitat Valenciana</t>
   </si>
   <si>
@@ -84,13 +72,7 @@
     <t>Madrid, Comunidad de</t>
   </si>
   <si>
-    <t>Murcia, Región de</t>
-  </si>
-  <si>
     <t>Navarra, Comunidad Foral de</t>
-  </si>
-  <si>
-    <t>País Vasco</t>
   </si>
   <si>
     <t>Rioja, La</t>
@@ -365,6 +347,27 @@
       <t xml:space="preserve">
 Este dataset presenta un conjunto de datos de las Tasas de variación de fallecidos en 2020 respecto al año anterior. Destacar que que 2020 fue el año del COVID y 1Ola, 2Ola, 3Ola corresponden a las semanas en las que se dieron dichas olas.</t>
     </r>
+  </si>
+  <si>
+    <t>30324 Estimación de Defunciones Semanales</t>
+  </si>
+  <si>
+    <t>Andalucia</t>
+  </si>
+  <si>
+    <t>Aragon</t>
+  </si>
+  <si>
+    <t>Castilla y Leon</t>
+  </si>
+  <si>
+    <t>Cataluna</t>
+  </si>
+  <si>
+    <t>Murcia, Region de</t>
+  </si>
+  <si>
+    <t>Pais Vasco</t>
   </si>
 </sst>
 </file>
@@ -495,7 +498,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="17">
+  <borders count="18">
     <border>
       <left/>
       <right/>
@@ -679,6 +682,21 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -688,7 +706,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="42">
+  <cellXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -766,6 +784,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
@@ -1117,93 +1138,93 @@
   <dimension ref="B2:G12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3:G12"/>
+      <selection activeCell="H19" sqref="H19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="2" spans="2:7" ht="16" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="3" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B3" s="33" t="s">
-        <v>101</v>
-      </c>
-      <c r="C3" s="34"/>
-      <c r="D3" s="34"/>
-      <c r="E3" s="34"/>
-      <c r="F3" s="34"/>
-      <c r="G3" s="35"/>
+      <c r="B3" s="34" t="s">
+        <v>95</v>
+      </c>
+      <c r="C3" s="35"/>
+      <c r="D3" s="35"/>
+      <c r="E3" s="35"/>
+      <c r="F3" s="35"/>
+      <c r="G3" s="36"/>
     </row>
     <row r="4" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B4" s="36"/>
-      <c r="C4" s="37"/>
-      <c r="D4" s="37"/>
-      <c r="E4" s="37"/>
-      <c r="F4" s="37"/>
-      <c r="G4" s="38"/>
+      <c r="B4" s="37"/>
+      <c r="C4" s="38"/>
+      <c r="D4" s="38"/>
+      <c r="E4" s="38"/>
+      <c r="F4" s="38"/>
+      <c r="G4" s="39"/>
     </row>
     <row r="5" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B5" s="36"/>
-      <c r="C5" s="37"/>
-      <c r="D5" s="37"/>
-      <c r="E5" s="37"/>
-      <c r="F5" s="37"/>
-      <c r="G5" s="38"/>
+      <c r="B5" s="37"/>
+      <c r="C5" s="38"/>
+      <c r="D5" s="38"/>
+      <c r="E5" s="38"/>
+      <c r="F5" s="38"/>
+      <c r="G5" s="39"/>
     </row>
     <row r="6" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B6" s="36"/>
-      <c r="C6" s="37"/>
-      <c r="D6" s="37"/>
-      <c r="E6" s="37"/>
-      <c r="F6" s="37"/>
-      <c r="G6" s="38"/>
+      <c r="B6" s="37"/>
+      <c r="C6" s="38"/>
+      <c r="D6" s="38"/>
+      <c r="E6" s="38"/>
+      <c r="F6" s="38"/>
+      <c r="G6" s="39"/>
     </row>
     <row r="7" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B7" s="36"/>
-      <c r="C7" s="37"/>
-      <c r="D7" s="37"/>
-      <c r="E7" s="37"/>
-      <c r="F7" s="37"/>
-      <c r="G7" s="38"/>
+      <c r="B7" s="37"/>
+      <c r="C7" s="38"/>
+      <c r="D7" s="38"/>
+      <c r="E7" s="38"/>
+      <c r="F7" s="38"/>
+      <c r="G7" s="39"/>
     </row>
     <row r="8" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B8" s="36"/>
-      <c r="C8" s="37"/>
-      <c r="D8" s="37"/>
-      <c r="E8" s="37"/>
-      <c r="F8" s="37"/>
-      <c r="G8" s="38"/>
+      <c r="B8" s="37"/>
+      <c r="C8" s="38"/>
+      <c r="D8" s="38"/>
+      <c r="E8" s="38"/>
+      <c r="F8" s="38"/>
+      <c r="G8" s="39"/>
     </row>
     <row r="9" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B9" s="36"/>
-      <c r="C9" s="37"/>
-      <c r="D9" s="37"/>
-      <c r="E9" s="37"/>
-      <c r="F9" s="37"/>
-      <c r="G9" s="38"/>
+      <c r="B9" s="37"/>
+      <c r="C9" s="38"/>
+      <c r="D9" s="38"/>
+      <c r="E9" s="38"/>
+      <c r="F9" s="38"/>
+      <c r="G9" s="39"/>
     </row>
     <row r="10" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B10" s="36"/>
-      <c r="C10" s="37"/>
-      <c r="D10" s="37"/>
-      <c r="E10" s="37"/>
-      <c r="F10" s="37"/>
-      <c r="G10" s="38"/>
+      <c r="B10" s="37"/>
+      <c r="C10" s="38"/>
+      <c r="D10" s="38"/>
+      <c r="E10" s="38"/>
+      <c r="F10" s="38"/>
+      <c r="G10" s="39"/>
     </row>
     <row r="11" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B11" s="36"/>
-      <c r="C11" s="37"/>
-      <c r="D11" s="37"/>
-      <c r="E11" s="37"/>
-      <c r="F11" s="37"/>
-      <c r="G11" s="38"/>
+      <c r="B11" s="37"/>
+      <c r="C11" s="38"/>
+      <c r="D11" s="38"/>
+      <c r="E11" s="38"/>
+      <c r="F11" s="38"/>
+      <c r="G11" s="39"/>
     </row>
     <row r="12" spans="2:7" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B12" s="39"/>
-      <c r="C12" s="40"/>
-      <c r="D12" s="40"/>
-      <c r="E12" s="40"/>
-      <c r="F12" s="40"/>
-      <c r="G12" s="41"/>
+      <c r="B12" s="40"/>
+      <c r="C12" s="41"/>
+      <c r="D12" s="41"/>
+      <c r="E12" s="41"/>
+      <c r="F12" s="41"/>
+      <c r="G12" s="42"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -1218,7 +1239,7 @@
   <dimension ref="A1:F21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F19" sqref="F19"/>
+      <selection activeCell="A21" sqref="A21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1240,18 +1261,18 @@
         <v>0</v>
       </c>
       <c r="D1" s="29" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="E1" s="29" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="F1" s="29" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
     </row>
     <row r="2" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A2" s="30" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="B2" s="19">
         <v>26.02</v>
@@ -1271,7 +1292,7 @@
     </row>
     <row r="3" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A3" s="30" t="s">
-        <v>3</v>
+        <v>97</v>
       </c>
       <c r="B3" s="19">
         <v>4.49</v>
@@ -1291,7 +1312,7 @@
     </row>
     <row r="4" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A4" s="30" t="s">
-        <v>4</v>
+        <v>98</v>
       </c>
       <c r="B4" s="19">
         <v>22.26</v>
@@ -1311,7 +1332,7 @@
     </row>
     <row r="5" spans="1:6" ht="32" x14ac:dyDescent="0.2">
       <c r="A5" s="30" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="B5" s="19">
         <v>9.84</v>
@@ -1331,7 +1352,7 @@
     </row>
     <row r="6" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A6" s="30" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="B6" s="19">
         <v>1.88</v>
@@ -1351,7 +1372,7 @@
     </row>
     <row r="7" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A7" s="30" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="B7" s="19">
         <v>2.2200000000000002</v>
@@ -1371,7 +1392,7 @@
     </row>
     <row r="8" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A8" s="30" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B8" s="19">
         <v>8.18</v>
@@ -1391,7 +1412,7 @@
     </row>
     <row r="9" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A9" s="30" t="s">
-        <v>9</v>
+        <v>99</v>
       </c>
       <c r="B9" s="19">
         <v>34.49</v>
@@ -1411,7 +1432,7 @@
     </row>
     <row r="10" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A10" s="30" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="B10" s="19">
         <v>58.79</v>
@@ -1431,7 +1452,7 @@
     </row>
     <row r="11" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A11" s="30" t="s">
-        <v>11</v>
+        <v>100</v>
       </c>
       <c r="B11" s="19">
         <v>41.34</v>
@@ -1451,7 +1472,7 @@
     </row>
     <row r="12" spans="1:6" ht="32" x14ac:dyDescent="0.2">
       <c r="A12" s="30" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="B12" s="19">
         <v>7.18</v>
@@ -1471,7 +1492,7 @@
     </row>
     <row r="13" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A13" s="30" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="B13" s="19">
         <v>14.89</v>
@@ -1491,7 +1512,7 @@
     </row>
     <row r="14" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A14" s="30" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="B14" s="19">
         <v>5.56</v>
@@ -1511,7 +1532,7 @@
     </row>
     <row r="15" spans="1:6" ht="32" x14ac:dyDescent="0.2">
       <c r="A15" s="30" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="B15" s="19">
         <v>82.48</v>
@@ -1531,7 +1552,7 @@
     </row>
     <row r="16" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A16" s="30" t="s">
-        <v>16</v>
+        <v>101</v>
       </c>
       <c r="B16" s="19">
         <v>-0.75</v>
@@ -1551,7 +1572,7 @@
     </row>
     <row r="17" spans="1:6" ht="32" x14ac:dyDescent="0.2">
       <c r="A17" s="30" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="B17" s="19">
         <v>35.69</v>
@@ -1571,7 +1592,7 @@
     </row>
     <row r="18" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A18" s="30" t="s">
-        <v>18</v>
+        <v>102</v>
       </c>
       <c r="B18" s="19">
         <v>16.55</v>
@@ -1591,7 +1612,7 @@
     </row>
     <row r="19" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A19" s="30" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="B19" s="19">
         <v>24.83</v>
@@ -1611,7 +1632,7 @@
     </row>
     <row r="20" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A20" s="30" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="B20" s="19">
         <v>23.5</v>
@@ -1631,7 +1652,7 @@
     </row>
     <row r="21" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A21" s="32" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="B21" s="19">
         <v>20.83</v>
@@ -1658,8 +1679,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A8299C2B-CE50-424F-AE07-5716E5166FB9}">
   <dimension ref="A1:J7"/>
   <sheetViews>
-    <sheetView zoomScale="119" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+    <sheetView topLeftCell="B1" zoomScale="119" workbookViewId="0">
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1678,34 +1699,34 @@
   <sheetData>
     <row r="1" spans="1:10" ht="35" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="D1" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="E1" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="F1" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="H1" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="B1" s="5" t="s">
+      <c r="I1" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="C1" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="D1" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="E1" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="F1" s="4" t="s">
-        <v>53</v>
-      </c>
-      <c r="G1" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="H1" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="I1" s="3" t="s">
-        <v>33</v>
-      </c>
       <c r="J1" s="2" t="s">
-        <v>55</v>
+        <v>49</v>
       </c>
     </row>
     <row r="2" spans="1:10" ht="16" x14ac:dyDescent="0.2">
@@ -1713,16 +1734,16 @@
         <v>2</v>
       </c>
       <c r="B2" s="9" t="s">
-        <v>34</v>
+        <v>28</v>
       </c>
       <c r="C2" s="6" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
       <c r="D2" s="6" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
       <c r="E2" s="9" t="s">
-        <v>36</v>
+        <v>30</v>
       </c>
       <c r="F2" s="7"/>
       <c r="G2" s="10"/>
@@ -1735,29 +1756,29 @@
         <v>1</v>
       </c>
       <c r="B3" s="11" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
       <c r="C3" s="11" t="s">
-        <v>47</v>
+        <v>41</v>
       </c>
       <c r="D3" s="9" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
       <c r="E3" s="9" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
       <c r="F3" s="11" t="s">
-        <v>37</v>
+        <v>96</v>
       </c>
       <c r="G3" s="11"/>
       <c r="H3" s="11" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
       <c r="I3" s="11">
         <v>35177</v>
       </c>
       <c r="J3" s="12" t="s">
-        <v>42</v>
+        <v>36</v>
       </c>
     </row>
     <row r="4" spans="1:10" ht="48" x14ac:dyDescent="0.2">
@@ -1765,119 +1786,119 @@
         <v>0</v>
       </c>
       <c r="B4" s="11" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
       <c r="C4" s="11" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="D4" s="9" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
       <c r="E4" s="9" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
       <c r="F4" s="11" t="s">
-        <v>37</v>
+        <v>96</v>
       </c>
       <c r="G4" s="11"/>
       <c r="H4" s="11" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
       <c r="I4" s="11">
         <v>35177</v>
       </c>
       <c r="J4" s="12" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
     </row>
     <row r="5" spans="1:10" ht="80" x14ac:dyDescent="0.2">
       <c r="A5" s="11" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="B5" s="11" t="s">
-        <v>44</v>
+        <v>38</v>
       </c>
       <c r="C5" s="11" t="s">
-        <v>49</v>
+        <v>43</v>
       </c>
       <c r="D5" s="9" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
       <c r="E5" s="9" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
       <c r="F5" s="11" t="s">
-        <v>37</v>
+        <v>96</v>
       </c>
       <c r="G5" s="11"/>
       <c r="H5" s="11" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
       <c r="I5" s="11">
         <v>35177</v>
       </c>
       <c r="J5" s="12" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
     </row>
     <row r="6" spans="1:10" ht="80" x14ac:dyDescent="0.2">
       <c r="A6" s="11" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="B6" s="11" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="C6" s="11" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
       <c r="D6" s="9" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
       <c r="E6" s="9" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
       <c r="F6" s="11" t="s">
-        <v>37</v>
+        <v>96</v>
       </c>
       <c r="G6" s="11"/>
       <c r="H6" s="11" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
       <c r="I6" s="11">
         <v>35177</v>
       </c>
       <c r="J6" s="12" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
     </row>
     <row r="7" spans="1:10" ht="81" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A7" s="13" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="B7" s="13" t="s">
-        <v>46</v>
+        <v>40</v>
       </c>
       <c r="C7" s="13" t="s">
-        <v>51</v>
+        <v>45</v>
       </c>
       <c r="D7" s="14" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
       <c r="E7" s="14" t="s">
-        <v>38</v>
-      </c>
-      <c r="F7" s="13" t="s">
-        <v>37</v>
+        <v>32</v>
+      </c>
+      <c r="F7" s="33" t="s">
+        <v>96</v>
       </c>
       <c r="G7" s="13"/>
       <c r="H7" s="13" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
       <c r="I7" s="13">
         <v>35177</v>
       </c>
       <c r="J7" s="15" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
     </row>
   </sheetData>
@@ -1895,7 +1916,7 @@
   <dimension ref="A1:B45"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E22" sqref="E22"/>
+      <selection activeCell="D27" sqref="D27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1906,15 +1927,15 @@
   <sheetData>
     <row r="1" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A1" s="16" t="s">
-        <v>56</v>
+        <v>50</v>
       </c>
       <c r="B1" s="17" t="s">
-        <v>100</v>
+        <v>94</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" s="18" t="s">
-        <v>57</v>
+        <v>51</v>
       </c>
       <c r="B2" s="19">
         <v>1</v>
@@ -1922,7 +1943,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" s="18" t="s">
-        <v>58</v>
+        <v>52</v>
       </c>
       <c r="B3" s="19">
         <v>0</v>
@@ -1930,7 +1951,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" s="18" t="s">
-        <v>59</v>
+        <v>53</v>
       </c>
       <c r="B4" s="19">
         <v>0</v>
@@ -1938,7 +1959,7 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" s="20" t="s">
-        <v>60</v>
+        <v>54</v>
       </c>
       <c r="B5" s="19">
         <v>0</v>
@@ -1946,7 +1967,7 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" s="21" t="s">
-        <v>61</v>
+        <v>55</v>
       </c>
       <c r="B6" s="19">
         <v>1</v>
@@ -1954,7 +1975,7 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7" s="21" t="s">
-        <v>62</v>
+        <v>56</v>
       </c>
       <c r="B7" s="19">
         <v>1</v>
@@ -1962,7 +1983,7 @@
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A8" s="21" t="s">
-        <v>63</v>
+        <v>57</v>
       </c>
       <c r="B8" s="19">
         <v>1</v>
@@ -1970,7 +1991,7 @@
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A9" s="21" t="s">
-        <v>64</v>
+        <v>58</v>
       </c>
       <c r="B9" s="19">
         <v>0</v>
@@ -1978,7 +1999,7 @@
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A10" s="21" t="s">
-        <v>65</v>
+        <v>59</v>
       </c>
       <c r="B10" s="19">
         <v>0</v>
@@ -1986,7 +2007,7 @@
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A11" s="22" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
       <c r="B11" s="19">
         <v>1</v>
@@ -1994,7 +2015,7 @@
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A12" s="22" t="s">
-        <v>67</v>
+        <v>61</v>
       </c>
       <c r="B12" s="19">
         <v>0</v>
@@ -2002,7 +2023,7 @@
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A13" s="22" t="s">
-        <v>68</v>
+        <v>62</v>
       </c>
       <c r="B13" s="19">
         <v>0</v>
@@ -2010,7 +2031,7 @@
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A14" s="22" t="s">
-        <v>69</v>
+        <v>63</v>
       </c>
       <c r="B14" s="19">
         <v>0</v>
@@ -2018,7 +2039,7 @@
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A15" s="22" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
       <c r="B15" s="19">
         <v>0</v>
@@ -2026,7 +2047,7 @@
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A16" s="22" t="s">
-        <v>71</v>
+        <v>65</v>
       </c>
       <c r="B16" s="19">
         <v>0</v>
@@ -2034,7 +2055,7 @@
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A17" s="22" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
       <c r="B17" s="19">
         <v>0</v>
@@ -2042,7 +2063,7 @@
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A18" s="22" t="s">
-        <v>73</v>
+        <v>67</v>
       </c>
       <c r="B18" s="19">
         <v>0</v>
@@ -2050,7 +2071,7 @@
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A19" s="22" t="s">
-        <v>74</v>
+        <v>68</v>
       </c>
       <c r="B19" s="19">
         <v>0</v>
@@ -2058,7 +2079,7 @@
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A20" s="23" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
       <c r="B20" s="19">
         <v>0</v>
@@ -2066,7 +2087,7 @@
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A21" s="23" t="s">
-        <v>76</v>
+        <v>70</v>
       </c>
       <c r="B21" s="19">
         <v>0</v>
@@ -2074,7 +2095,7 @@
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A22" s="23" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
       <c r="B22" s="19">
         <v>1</v>
@@ -2082,7 +2103,7 @@
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A23" s="23" t="s">
-        <v>78</v>
+        <v>72</v>
       </c>
       <c r="B23" s="19">
         <v>0</v>
@@ -2090,7 +2111,7 @@
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A24" s="23" t="s">
-        <v>79</v>
+        <v>73</v>
       </c>
       <c r="B24" s="19">
         <v>0</v>
@@ -2098,7 +2119,7 @@
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A25" s="23" t="s">
-        <v>80</v>
+        <v>74</v>
       </c>
       <c r="B25" s="19">
         <v>0</v>
@@ -2106,7 +2127,7 @@
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A26" s="23" t="s">
-        <v>81</v>
+        <v>75</v>
       </c>
       <c r="B26" s="19">
         <v>0</v>
@@ -2114,7 +2135,7 @@
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A27" s="23" t="s">
-        <v>82</v>
+        <v>76</v>
       </c>
       <c r="B27" s="19">
         <v>0</v>
@@ -2122,23 +2143,23 @@
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A28" s="23" t="s">
-        <v>83</v>
+        <v>77</v>
       </c>
       <c r="B28" s="19">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A29" s="23" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
       <c r="B29" s="19">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A30" s="24" t="s">
-        <v>84</v>
+        <v>78</v>
       </c>
       <c r="B30" s="19">
         <v>0</v>
@@ -2146,7 +2167,7 @@
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A31" s="24" t="s">
-        <v>85</v>
+        <v>79</v>
       </c>
       <c r="B31" s="19">
         <v>0</v>
@@ -2154,7 +2175,7 @@
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A32" s="24" t="s">
-        <v>86</v>
+        <v>80</v>
       </c>
       <c r="B32" s="19">
         <v>0</v>
@@ -2162,7 +2183,7 @@
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A33" s="24" t="s">
-        <v>87</v>
+        <v>81</v>
       </c>
       <c r="B33" s="19">
         <v>0</v>
@@ -2170,7 +2191,7 @@
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A34" s="24" t="s">
-        <v>88</v>
+        <v>82</v>
       </c>
       <c r="B34" s="19">
         <v>0</v>
@@ -2178,7 +2199,7 @@
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A35" s="25" t="s">
-        <v>89</v>
+        <v>83</v>
       </c>
       <c r="B35" s="19">
         <v>1</v>
@@ -2186,7 +2207,7 @@
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A36" s="25" t="s">
-        <v>90</v>
+        <v>84</v>
       </c>
       <c r="B36" s="19">
         <v>1</v>
@@ -2194,7 +2215,7 @@
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A37" s="25" t="s">
-        <v>91</v>
+        <v>85</v>
       </c>
       <c r="B37" s="19">
         <v>0</v>
@@ -2202,7 +2223,7 @@
     </row>
     <row r="38" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A38" s="26" t="s">
-        <v>92</v>
+        <v>86</v>
       </c>
       <c r="B38" s="8">
         <v>0</v>
@@ -2210,7 +2231,7 @@
     </row>
     <row r="39" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A39" s="26" t="s">
-        <v>93</v>
+        <v>87</v>
       </c>
       <c r="B39" s="8">
         <v>0</v>
@@ -2218,7 +2239,7 @@
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A40" s="27" t="s">
-        <v>94</v>
+        <v>88</v>
       </c>
       <c r="B40" s="8">
         <v>0</v>
@@ -2226,7 +2247,7 @@
     </row>
     <row r="41" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A41" s="26" t="s">
-        <v>95</v>
+        <v>89</v>
       </c>
       <c r="B41" s="8">
         <v>0</v>
@@ -2234,7 +2255,7 @@
     </row>
     <row r="42" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A42" s="26" t="s">
-        <v>96</v>
+        <v>90</v>
       </c>
       <c r="B42" s="8">
         <v>0</v>
@@ -2242,7 +2263,7 @@
     </row>
     <row r="43" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A43" s="26" t="s">
-        <v>97</v>
+        <v>91</v>
       </c>
       <c r="B43" s="8">
         <v>1</v>
@@ -2250,7 +2271,7 @@
     </row>
     <row r="44" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A44" s="26" t="s">
-        <v>98</v>
+        <v>92</v>
       </c>
       <c r="B44" s="8">
         <v>0</v>
@@ -2258,7 +2279,7 @@
     </row>
     <row r="45" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A45" s="26" t="s">
-        <v>99</v>
+        <v>93</v>
       </c>
       <c r="B45" s="8">
         <v>0</v>

</xml_diff>